<commit_message>
bug fix:runner put case need lock; result.result should be RESULT_GROUP
</commit_message>
<xml_diff>
--- a/testcases/test.xlsx
+++ b/testcases/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2539" uniqueCount="474">
   <si>
     <t>id</t>
   </si>
@@ -3093,6 +3093,18 @@
   <si>
     <t>template</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{}123</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.GetCityWeather</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3.GetCityWeather</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3539,9 +3551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomLeft" activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="49.9" customHeight="1"/>
@@ -3698,7 +3710,7 @@
         <v>20</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>469</v>
+        <v>147</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>397</v>
@@ -3773,7 +3785,7 @@
         <v>20</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>469</v>
+        <v>147</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>397</v>
@@ -3799,7 +3811,9 @@
       <c r="X3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y3" s="3"/>
+      <c r="Y3" s="3" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="4" spans="1:25" ht="49.9" customHeight="1">
       <c r="A4" s="1">
@@ -3848,7 +3862,7 @@
         <v>20</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>469</v>
+        <v>147</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>397</v>
@@ -3923,7 +3937,7 @@
         <v>20</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>469</v>
+        <v>147</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>397</v>
@@ -3949,7 +3963,9 @@
       <c r="X5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y5" s="3"/>
+      <c r="Y5" s="3" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="6" spans="1:25" ht="49.9" customHeight="1">
       <c r="A6" s="1">
@@ -3998,7 +4014,7 @@
         <v>20</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>469</v>
+        <v>147</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>397</v>
@@ -4027,49 +4043,153 @@
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="1:25" ht="49.9" customHeight="1">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="3"/>
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="1:25" ht="49.9" customHeight="1">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="3"/>
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="Y8" s="3"/>
     </row>
     <row r="9" spans="1:25" ht="49.9" customHeight="1">
@@ -6609,9 +6729,13 @@
     <hyperlink ref="I5" r:id="rId8" display="https://api-server-corpus.zhan.com/toefl/filtrate-paper"/>
     <hyperlink ref="J6" r:id="rId9" display="http://192.168.41.106:8093/token"/>
     <hyperlink ref="I6" r:id="rId10" display="https://api-server-corpus.zhan.com/toefl/filtrate-paper"/>
+    <hyperlink ref="J7" r:id="rId11" display="http://192.168.41.106:8093/token"/>
+    <hyperlink ref="I7" r:id="rId12" display="https://api-server-corpus.zhan.com/toefl/filtrate-paper"/>
+    <hyperlink ref="J8" r:id="rId13" display="http://192.168.41.106:8093/token"/>
+    <hyperlink ref="I8" r:id="rId14" display="https://api-server-corpus.zhan.com/toefl/filtrate-paper"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
complete common config #12
</commit_message>
<xml_diff>
--- a/testcases/test.xlsx
+++ b/testcases/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="testcases" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2539" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="474">
   <si>
     <t>id</t>
   </si>
@@ -3551,9 +3551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="49.9" customHeight="1"/>
@@ -6866,35 +6866,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>458</v>
       </c>
       <c r="B1" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>470</v>
       </c>
       <c r="B2" t="s">
         <v>470</v>
       </c>
+      <c r="C2" s="10" t="s">
+        <v>467</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://api-server-corpus.zhan.com/toefl/filtrate-paper"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>